<commit_message>
rebuild DB and add new forms for adding to db
</commit_message>
<xml_diff>
--- a/database_build/schema.xlsx
+++ b/database_build/schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LifeHistory\database_build\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LifeHistory\Lifehistory\database_build\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="86">
   <si>
     <t>TABLE</t>
   </si>
@@ -255,6 +255,33 @@
   </si>
   <si>
     <t>citation_numerictraits</t>
+  </si>
+  <si>
+    <t>traitnames</t>
+  </si>
+  <si>
+    <t>trtnmid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTEGER </t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>tr_value</t>
+  </si>
+  <si>
+    <t>tr_name</t>
+  </si>
+  <si>
+    <t>foraging</t>
+  </si>
+  <si>
+    <t>forid</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -624,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +702,9 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -686,6 +716,9 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -697,6 +730,9 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -708,6 +744,9 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
+      <c r="E6" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -716,6 +755,9 @@
       <c r="C7" t="s">
         <v>65</v>
       </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -727,6 +769,9 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -737,6 +782,9 @@
       </c>
       <c r="D9" t="s">
         <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,6 +809,9 @@
       <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -772,6 +823,9 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
+      <c r="E13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
@@ -783,6 +837,9 @@
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="E14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -796,7 +853,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -809,8 +866,11 @@
       <c r="D17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -820,64 +880,88 @@
       <c r="D18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>39</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>40</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>43</v>
       </c>
@@ -885,8 +969,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
@@ -899,8 +983,11 @@
       <c r="D28" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>12</v>
       </c>
@@ -910,8 +997,11 @@
       <c r="D29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>46</v>
       </c>
@@ -921,8 +1011,11 @@
       <c r="D30" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>47</v>
       </c>
@@ -932,213 +1025,283 @@
       <c r="D31" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="E31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="E36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>13</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D37" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="E37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="D38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D39" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>62</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B44" t="s">
         <v>22</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>38</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D44" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="E44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>12</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C45" t="s">
         <v>13</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D45" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="E45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>21</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C46" t="s">
         <v>52</v>
       </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>53</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C47" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="E47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>54</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C48" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="E48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>55</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="E49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C50" t="s">
         <v>10</v>
       </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C51" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="E51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>24</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C53" t="s">
         <v>25</v>
       </c>
-      <c r="D46" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>26</v>
-      </c>
-      <c r="C47" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C53" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>24</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
@@ -1147,132 +1310,160 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>26</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C63" t="s">
         <v>25</v>
       </c>
-      <c r="D55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>31</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B65" t="s">
         <v>29</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C65" t="s">
         <v>30</v>
-      </c>
-      <c r="D57" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>33</v>
-      </c>
-      <c r="C58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D58" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" t="s">
-        <v>38</v>
-      </c>
-      <c r="D61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" t="s">
-        <v>38</v>
       </c>
       <c r="D65" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="D66" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E66" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C67" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D67" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
         <v>64</v>
@@ -1283,19 +1474,25 @@
       <c r="D69" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D70" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>29</v>
       </c>
@@ -1306,6 +1503,249 @@
         <v>32</v>
       </c>
     </row>
+    <row r="72" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>69</v>
+      </c>
+      <c r="E74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>75</v>
+      </c>
+      <c r="E78" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" t="s">
+        <v>30</v>
+      </c>
+      <c r="D79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" t="s">
+        <v>30</v>
+      </c>
+      <c r="D84" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" t="s">
+        <v>38</v>
+      </c>
+      <c r="D87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" t="s">
+        <v>20</v>
+      </c>
+      <c r="E89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" t="s">
+        <v>30</v>
+      </c>
+      <c r="D90" t="s">
+        <v>32</v>
+      </c>
+      <c r="E90" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" t="s">
+        <v>25</v>
+      </c>
+      <c r="D91" t="s">
+        <v>20</v>
+      </c>
+      <c r="E91" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="C92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Reconfig database structure and completed data entry forms
</commit_message>
<xml_diff>
--- a/database_build/schema.xlsx
+++ b/database_build/schema.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="85">
   <si>
     <t>TABLE</t>
   </si>
@@ -56,18 +56,12 @@
     <t>genus</t>
   </si>
   <si>
-    <t>character(20)</t>
-  </si>
-  <si>
     <t>subspecies</t>
   </si>
   <si>
     <t>species_id</t>
   </si>
   <si>
-    <t>character(40)</t>
-  </si>
-  <si>
     <t>synonyms</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>character(30)</t>
-  </si>
-  <si>
     <t>dt</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
     <t>cite_id</t>
   </si>
   <si>
-    <t>character(15)</t>
-  </si>
-  <si>
     <t>citation</t>
   </si>
   <si>
@@ -170,9 +158,6 @@
     <t>breeding_distribution</t>
   </si>
   <si>
-    <t>character(10)</t>
-  </si>
-  <si>
     <t>nlid</t>
   </si>
   <si>
@@ -182,9 +167,6 @@
     <t>nest_location</t>
   </si>
   <si>
-    <t>character(60)</t>
-  </si>
-  <si>
     <t>mean</t>
   </si>
   <si>
@@ -209,27 +191,12 @@
     <t>common_name</t>
   </si>
   <si>
-    <t>character(100)</t>
-  </si>
-  <si>
     <t>numeric_traits</t>
   </si>
   <si>
-    <t>species_citation</t>
-  </si>
-  <si>
     <t>relation_id</t>
   </si>
   <si>
-    <t>character(50)</t>
-  </si>
-  <si>
-    <t>character(300)</t>
-  </si>
-  <si>
-    <t>character(4)</t>
-  </si>
-  <si>
     <t>numeric(10,4)</t>
   </si>
   <si>
@@ -248,15 +215,9 @@
     <t>value</t>
   </si>
   <si>
-    <t>citation_othertraits</t>
-  </si>
-  <si>
     <t>NOT NULL REFERENCES other_traits (trtid)</t>
   </si>
   <si>
-    <t>citation_numerictraits</t>
-  </si>
-  <si>
     <t>traitnames</t>
   </si>
   <si>
@@ -282,6 +243,42 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>character varying(20)</t>
+  </si>
+  <si>
+    <t>character varying(50)</t>
+  </si>
+  <si>
+    <t>character varying(40)</t>
+  </si>
+  <si>
+    <t>character varying(300)</t>
+  </si>
+  <si>
+    <t>character varying(100)</t>
+  </si>
+  <si>
+    <t>character varying(4)</t>
+  </si>
+  <si>
+    <t>character varying(60)</t>
+  </si>
+  <si>
+    <t>character varying(10)</t>
+  </si>
+  <si>
+    <t>character varying(30)</t>
+  </si>
+  <si>
+    <t>character varying(25)</t>
+  </si>
+  <si>
+    <t>citation_numerictrait_species</t>
+  </si>
+  <si>
+    <t>citation_othertraits_species</t>
   </si>
 </sst>
 </file>
@@ -651,18 +648,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E92"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -697,13 +695,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,13 +709,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,13 +723,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,1013 +737,998 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E38" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E41" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E44" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E47" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D50" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D52" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E52" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D53" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D56" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D57" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E58" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="E59" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E60" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C61" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D61" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E61" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D62" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E62" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D63" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C65" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D65" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E65" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E66" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D67" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D69" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E69" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E70" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="D71" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" t="s">
-        <v>64</v>
-      </c>
-      <c r="C73" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73" t="s">
-        <v>27</v>
-      </c>
-      <c r="E73" t="s">
-        <v>85</v>
-      </c>
-    </row>
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" t="s">
+        <v>75</v>
+      </c>
+      <c r="D72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>84</v>
+      </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D74" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="E74" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C75" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D75" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>63</v>
+      </c>
+      <c r="E75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+      <c r="C76" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>74</v>
-      </c>
       <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" t="s">
+        <v>75</v>
+      </c>
+      <c r="D77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>64</v>
       </c>
-      <c r="C77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" t="s">
-        <v>27</v>
-      </c>
-      <c r="E77" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="B79" t="s">
+        <v>65</v>
+      </c>
+      <c r="C79" t="s">
+        <v>66</v>
+      </c>
+      <c r="D79" t="s">
+        <v>24</v>
+      </c>
+      <c r="E79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" t="s">
         <v>75</v>
       </c>
-      <c r="E78" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>29</v>
-      </c>
-      <c r="C79" t="s">
-        <v>30</v>
-      </c>
-      <c r="D79" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D80" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>77</v>
-      </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C81" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D81" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E81" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="D82" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E82" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="D83" t="s">
-        <v>20</v>
-      </c>
-      <c r="E83" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" t="s">
-        <v>30</v>
-      </c>
-      <c r="D84" t="s">
-        <v>20</v>
-      </c>
-      <c r="E84" t="s">
-        <v>85</v>
-      </c>
-    </row>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>70</v>
+      </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C85" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D85" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>24</v>
+      </c>
+      <c r="E85" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" t="s">
+        <v>75</v>
+      </c>
+      <c r="D86" t="s">
+        <v>25</v>
+      </c>
+      <c r="E86" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>83</v>
-      </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C87" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="D87" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E87" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="D88" t="s">
         <v>28</v>
       </c>
       <c r="E88" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="D89" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E89" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C90" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="D90" t="s">
-        <v>32</v>
-      </c>
-      <c r="E90" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>24</v>
-      </c>
-      <c r="C91" t="s">
-        <v>25</v>
-      </c>
-      <c r="D91" t="s">
-        <v>20</v>
-      </c>
-      <c r="E91" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>26</v>
-      </c>
-      <c r="C92" t="s">
-        <v>25</v>
-      </c>
-      <c r="D92" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>